<commit_message>
Iteration 1 Plan 1 Plan
</commit_message>
<xml_diff>
--- a/Project Plan/Detailed Project Plan.xlsx
+++ b/Project Plan/Detailed Project Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
   <si>
     <t>Iteration</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Reports</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Gary</t>
   </si>
 </sst>
 </file>
@@ -233,12 +239,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -546,7 +552,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G40"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,22 +589,22 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
         <v>0</v>
       </c>
       <c r="G2" t="s">
@@ -606,18 +612,18 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" t="s">
@@ -625,18 +631,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" t="s">
@@ -644,246 +650,278 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
         <v>4</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="D8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+      <c r="F13" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <v>1</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1">
         <v>3</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <v>2</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2">
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2">
-        <v>2</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
         <v>1</v>
       </c>
       <c r="H20" t="s">
@@ -894,16 +932,18 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
         <v>2</v>
       </c>
       <c r="H21">
@@ -916,234 +956,234 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
+      <c r="C22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
         <v>3</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3">
-        <v>1</v>
-      </c>
-      <c r="F24" s="3">
+      <c r="C24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
+      <c r="C26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
         <v>3</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3">
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3">
-        <v>2</v>
-      </c>
-      <c r="F29" s="3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3">
-        <v>1</v>
-      </c>
-      <c r="F30" s="3">
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="F30" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2">
         <v>3</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3">
+      <c r="C32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3">
-        <v>1</v>
-      </c>
-      <c r="F34" s="3">
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2">
         <v>3</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="2">
         <v>3</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H35" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3">
-        <v>1</v>
-      </c>
-      <c r="F36" s="3">
+      <c r="C36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2">
         <v>1</v>
       </c>
       <c r="H36" t="s">
@@ -1154,16 +1194,16 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3">
-        <v>2</v>
-      </c>
-      <c r="F37" s="3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
         <v>2</v>
       </c>
       <c r="H37">
@@ -1176,38 +1216,38 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>3</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4">
-        <v>2</v>
-      </c>
-      <c r="F38" s="4">
-        <v>2</v>
-      </c>
-      <c r="H38" s="1" t="s">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3">
+        <v>2</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I38" s="1"/>
+      <c r="I38" s="4"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4" t="s">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3">
         <v>15</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="3">
         <v>15</v>
       </c>
       <c r="H39" t="s">
@@ -1218,16 +1258,16 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4" t="s">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3">
         <v>15</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="3">
         <v>15</v>
       </c>
       <c r="H40">

</xml_diff>

<commit_message>
Modified Create and Add Project
</commit_message>
<xml_diff>
--- a/Project Plan/Detailed Project Plan.xlsx
+++ b/Project Plan/Detailed Project Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t>Iteration</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Team</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>Dan</t>
@@ -552,7 +549,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,8 +604,9 @@
       <c r="F2" s="1">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G41" si="0">IF(F2=0,"Done", "")</f>
+        <v>Done</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -618,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -626,8 +624,9 @@
       <c r="F3" s="1">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -645,20 +644,21 @@
       <c r="F4" s="1">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -666,18 +666,19 @@
       <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -685,18 +686,19 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" t="s">
-        <v>12</v>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -704,20 +706,21 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" t="s">
-        <v>12</v>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -725,18 +728,19 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-      <c r="G8" t="s">
-        <v>12</v>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -744,54 +748,63 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="1">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -799,18 +812,19 @@
       <c r="F12" s="1">
         <v>0</v>
       </c>
-      <c r="G12" t="s">
-        <v>12</v>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -818,104 +832,125 @@
       <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
-        <v>12</v>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Done</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
       </c>
       <c r="F17" s="1">
         <v>2</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -923,21 +958,25 @@
       <c r="F19" s="1">
         <v>2</v>
       </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H19" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -945,27 +984,35 @@
       <c r="F20" s="1">
         <v>1</v>
       </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" t="s">
         <v>38</v>
-      </c>
-      <c r="I20" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="H21">
         <f>SUM(E2:E21)</f>
@@ -973,7 +1020,7 @@
       </c>
       <c r="I21">
         <f>H21-SUM(F2:F21)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -981,10 +1028,10 @@
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
@@ -992,13 +1039,17 @@
       </c>
       <c r="F22" s="2">
         <v>1</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2">
@@ -1007,14 +1058,18 @@
       <c r="F23" s="2">
         <v>3</v>
       </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2">
@@ -1022,13 +1077,17 @@
       </c>
       <c r="F24" s="2">
         <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2">
@@ -1036,15 +1095,19 @@
       </c>
       <c r="F25" s="2">
         <v>1</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2">
@@ -1052,13 +1115,17 @@
       </c>
       <c r="F26" s="2">
         <v>1</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="27" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2">
@@ -1067,14 +1134,18 @@
       <c r="F27" s="2">
         <v>3</v>
       </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2">
@@ -1082,13 +1153,17 @@
       </c>
       <c r="F28" s="2">
         <v>1</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2">
@@ -1096,15 +1171,19 @@
       </c>
       <c r="F29" s="2">
         <v>2</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2">
@@ -1112,13 +1191,17 @@
       </c>
       <c r="F30" s="2">
         <v>1</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2">
@@ -1127,14 +1210,18 @@
       <c r="F31" s="2">
         <v>3</v>
       </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="32" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2">
@@ -1142,13 +1229,17 @@
       </c>
       <c r="F32" s="2">
         <v>1</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="33" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2">
@@ -1157,14 +1248,18 @@
       <c r="F33" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2">
@@ -1173,12 +1268,16 @@
       <c r="F34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2">
@@ -1187,18 +1286,22 @@
       <c r="F35" s="2">
         <v>3</v>
       </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2">
@@ -1207,18 +1310,22 @@
       <c r="F36" s="2">
         <v>1</v>
       </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
         <v>38</v>
       </c>
-      <c r="I36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2">
@@ -1226,6 +1333,10 @@
       </c>
       <c r="F37" s="2">
         <v>2</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="H37">
         <f>SUM(E22:E37)</f>
@@ -1236,15 +1347,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3">
@@ -1253,16 +1364,20 @@
       <c r="F38" s="3">
         <v>2</v>
       </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I38" s="4"/>
     </row>
-    <row r="39" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3">
@@ -1271,18 +1386,22 @@
       <c r="F39" s="3">
         <v>15</v>
       </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" t="s">
         <v>38</v>
       </c>
-      <c r="I39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3">
@@ -1291,6 +1410,10 @@
       <c r="F40" s="3">
         <v>15</v>
       </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="H40">
         <f>SUM(E38:E40)</f>
         <v>32</v>
@@ -1300,9 +1423,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41">
         <f>SUM(E2:E40)</f>
@@ -1310,7 +1433,11 @@
       </c>
       <c r="F41">
         <f>SUM(F2:F40)</f>
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated UMLs and DB
</commit_message>
<xml_diff>
--- a/Project Plan/Detailed Project Plan.xlsx
+++ b/Project Plan/Detailed Project Plan.xlsx
@@ -549,7 +549,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,11 +852,11 @@
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -872,11 +872,11 @@
         <v>3</v>
       </c>
       <c r="F15" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.35">
@@ -936,11 +936,11 @@
         <v>1</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -956,11 +956,11 @@
         <v>2</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Done</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>36</v>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="I21">
         <f>H21-SUM(F2:F21)</f>
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="F41">
         <f>SUM(F2:F40)</f>
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>

</xml_diff>